<commit_message>
Update files via changed
</commit_message>
<xml_diff>
--- a/maplib/files/input_files/input.xlsx
+++ b/maplib/files/input_files/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11016" tabRatio="1000" firstSheet="23" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11016" tabRatio="1000" firstSheet="21" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -12428,8 +12428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12618,7 +12618,7 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -13686,7 +13686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use json to compress files
</commit_message>
<xml_diff>
--- a/maplib/files/input_files/input.xlsx
+++ b/maplib/files/input_files/input.xlsx
@@ -4,47 +4,48 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11016" tabRatio="1000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11016" tabRatio="1000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="district name" sheetId="32" r:id="rId2"/>
-    <sheet name="water area name" sheetId="33" r:id="rId3"/>
-    <sheet name="Line 1" sheetId="2" r:id="rId4"/>
-    <sheet name="Line 2" sheetId="3" r:id="rId5"/>
-    <sheet name="Line 3" sheetId="4" r:id="rId6"/>
-    <sheet name="Line 4" sheetId="5" r:id="rId7"/>
-    <sheet name="Line 5" sheetId="6" r:id="rId8"/>
-    <sheet name="Line 6" sheetId="7" r:id="rId9"/>
-    <sheet name="Line 7" sheetId="8" r:id="rId10"/>
-    <sheet name="Line 8" sheetId="9" r:id="rId11"/>
-    <sheet name="Line 9" sheetId="10" r:id="rId12"/>
-    <sheet name="Line 10" sheetId="11" r:id="rId13"/>
-    <sheet name="Line 11" sheetId="13" r:id="rId14"/>
-    <sheet name="Line 12" sheetId="15" r:id="rId15"/>
-    <sheet name="Line 13" sheetId="16" r:id="rId16"/>
-    <sheet name="Line 14" sheetId="17" r:id="rId17"/>
-    <sheet name="Line 15" sheetId="18" r:id="rId18"/>
-    <sheet name="Line 16" sheetId="19" r:id="rId19"/>
-    <sheet name="Line 17" sheetId="20" r:id="rId20"/>
-    <sheet name="Line 18" sheetId="21" r:id="rId21"/>
-    <sheet name="Line 19" sheetId="22" r:id="rId22"/>
-    <sheet name="Line 20" sheetId="23" r:id="rId23"/>
-    <sheet name="Line 21" sheetId="24" r:id="rId24"/>
-    <sheet name="Line 23" sheetId="25" r:id="rId25"/>
-    <sheet name="Pujiang Line" sheetId="26" r:id="rId26"/>
-    <sheet name="Chongming Line" sheetId="27" r:id="rId27"/>
-    <sheet name="Airport Line" sheetId="29" r:id="rId28"/>
-    <sheet name="Jiamin Line" sheetId="30" r:id="rId29"/>
-    <sheet name="Maglev Line" sheetId="28" r:id="rId30"/>
-    <sheet name="Jinshan Railway" sheetId="31" r:id="rId31"/>
+    <sheet name="river name" sheetId="33" r:id="rId3"/>
+    <sheet name="lake name" sheetId="34" r:id="rId4"/>
+    <sheet name="Line 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Line 2" sheetId="3" r:id="rId6"/>
+    <sheet name="Line 3" sheetId="4" r:id="rId7"/>
+    <sheet name="Line 4" sheetId="5" r:id="rId8"/>
+    <sheet name="Line 5" sheetId="6" r:id="rId9"/>
+    <sheet name="Line 6" sheetId="7" r:id="rId10"/>
+    <sheet name="Line 7" sheetId="8" r:id="rId11"/>
+    <sheet name="Line 8" sheetId="9" r:id="rId12"/>
+    <sheet name="Line 9" sheetId="10" r:id="rId13"/>
+    <sheet name="Line 10" sheetId="11" r:id="rId14"/>
+    <sheet name="Line 11" sheetId="13" r:id="rId15"/>
+    <sheet name="Line 12" sheetId="15" r:id="rId16"/>
+    <sheet name="Line 13" sheetId="16" r:id="rId17"/>
+    <sheet name="Line 14" sheetId="17" r:id="rId18"/>
+    <sheet name="Line 15" sheetId="18" r:id="rId19"/>
+    <sheet name="Line 16" sheetId="19" r:id="rId20"/>
+    <sheet name="Line 17" sheetId="20" r:id="rId21"/>
+    <sheet name="Line 18" sheetId="21" r:id="rId22"/>
+    <sheet name="Line 19" sheetId="22" r:id="rId23"/>
+    <sheet name="Line 20" sheetId="23" r:id="rId24"/>
+    <sheet name="Line 21" sheetId="24" r:id="rId25"/>
+    <sheet name="Line 23" sheetId="25" r:id="rId26"/>
+    <sheet name="Pujiang Line" sheetId="26" r:id="rId27"/>
+    <sheet name="Chongming Line" sheetId="27" r:id="rId28"/>
+    <sheet name="Airport Line" sheetId="29" r:id="rId29"/>
+    <sheet name="Jiamin Line" sheetId="30" r:id="rId30"/>
+    <sheet name="Maglev Line" sheetId="28" r:id="rId31"/>
+    <sheet name="Jinshan Railway" sheetId="31" r:id="rId32"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="1184">
   <si>
     <t>Pujiang Line</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4432,6 +4433,14 @@
   </si>
   <si>
     <t>滴水湖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yangtze River</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5289,6 +5298,589 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="1">
+        <v>286</v>
+      </c>
+      <c r="E1" s="1">
+        <v>260</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="1">
+        <v>296</v>
+      </c>
+      <c r="E2" s="1">
+        <v>254</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="1">
+        <v>300</v>
+      </c>
+      <c r="E3" s="1">
+        <v>242</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="1">
+        <v>300</v>
+      </c>
+      <c r="E4" s="1">
+        <v>232</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D5" s="1">
+        <v>297</v>
+      </c>
+      <c r="E5" s="1">
+        <v>228</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="1">
+        <v>294</v>
+      </c>
+      <c r="E6" s="1">
+        <v>224</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="1">
+        <v>294</v>
+      </c>
+      <c r="E7" s="1">
+        <v>216</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="1">
+        <v>294</v>
+      </c>
+      <c r="E8" s="1">
+        <v>208</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="1">
+        <v>294</v>
+      </c>
+      <c r="E9" s="1">
+        <v>200</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="1">
+        <v>294</v>
+      </c>
+      <c r="E10" s="1">
+        <v>192</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="1">
+        <v>290</v>
+      </c>
+      <c r="E11" s="1">
+        <v>182</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12" s="1">
+        <v>284</v>
+      </c>
+      <c r="E12" s="1">
+        <v>176</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="1">
+        <v>278</v>
+      </c>
+      <c r="E13" s="1">
+        <v>172</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D14" s="1">
+        <v>271</v>
+      </c>
+      <c r="E14" s="1">
+        <v>172</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" s="1">
+        <v>265</v>
+      </c>
+      <c r="E15" s="1">
+        <v>172</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" s="1">
+        <v>258</v>
+      </c>
+      <c r="E16" s="1">
+        <v>172</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D17" s="1">
+        <v>251</v>
+      </c>
+      <c r="E17" s="1">
+        <v>172</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="1">
+        <v>240</v>
+      </c>
+      <c r="E18" s="1">
+        <v>164</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" s="1">
+        <v>234</v>
+      </c>
+      <c r="E19" s="1">
+        <v>156</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="1">
+        <v>234</v>
+      </c>
+      <c r="E20" s="1">
+        <v>150</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" s="1">
+        <v>231</v>
+      </c>
+      <c r="E21" s="1">
+        <v>145</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" s="1">
+        <v>227</v>
+      </c>
+      <c r="E22" s="1">
+        <v>141</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="1">
+        <v>222</v>
+      </c>
+      <c r="E23" s="1">
+        <v>136</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="1">
+        <v>218</v>
+      </c>
+      <c r="E24" s="1">
+        <v>128</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D25" s="1">
+        <v>218</v>
+      </c>
+      <c r="E25" s="1">
+        <v>119</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="1">
+        <v>212</v>
+      </c>
+      <c r="E26" s="1">
+        <v>116</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D27" s="1">
+        <v>205</v>
+      </c>
+      <c r="E27" s="1">
+        <v>116</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D28" s="1">
+        <v>198</v>
+      </c>
+      <c r="E28" s="1">
+        <v>116</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="1">
+        <v>192</v>
+      </c>
+      <c r="E29" s="1">
+        <v>120</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -5947,7 +6539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -6538,7 +7130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G35"/>
   <sheetViews>
@@ -7232,7 +7824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -7945,7 +8537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G41"/>
   <sheetViews>
@@ -8756,7 +9348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -9333,7 +9925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -10014,7 +10606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -10593,7 +11185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -11171,7 +11763,348 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C1">
+        <v>214</v>
+      </c>
+      <c r="D1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="D2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C4">
+        <v>167</v>
+      </c>
+      <c r="D4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C5">
+        <v>186</v>
+      </c>
+      <c r="D5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C6">
+        <v>130</v>
+      </c>
+      <c r="D6">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C7">
+        <v>237</v>
+      </c>
+      <c r="D7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C8">
+        <v>260</v>
+      </c>
+      <c r="D8">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C9">
+        <v>125</v>
+      </c>
+      <c r="D9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C10">
+        <v>184</v>
+      </c>
+      <c r="D10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C11">
+        <v>240</v>
+      </c>
+      <c r="D11">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C12">
+        <v>175</v>
+      </c>
+      <c r="D12">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C14">
+        <v>268</v>
+      </c>
+      <c r="D14">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C15">
+        <v>230</v>
+      </c>
+      <c r="D15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C16">
+        <v>336</v>
+      </c>
+      <c r="D16">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C17">
+        <v>336</v>
+      </c>
+      <c r="D17">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C18">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C19">
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C21">
+        <v>118</v>
+      </c>
+      <c r="D21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C22">
+        <v>364</v>
+      </c>
+      <c r="D22">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C23">
+        <v>332</v>
+      </c>
+      <c r="D23">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -11448,348 +12381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C1">
-        <v>214</v>
-      </c>
-      <c r="D1">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C2">
-        <v>150</v>
-      </c>
-      <c r="D2">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1147</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C3">
-        <v>130</v>
-      </c>
-      <c r="D3">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C4">
-        <v>167</v>
-      </c>
-      <c r="D4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C5">
-        <v>186</v>
-      </c>
-      <c r="D5">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>1148</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C6">
-        <v>130</v>
-      </c>
-      <c r="D6">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C7">
-        <v>237</v>
-      </c>
-      <c r="D7">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C8">
-        <v>260</v>
-      </c>
-      <c r="D8">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C9">
-        <v>125</v>
-      </c>
-      <c r="D9">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C10">
-        <v>184</v>
-      </c>
-      <c r="D10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>1152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1168</v>
-      </c>
-      <c r="C11">
-        <v>240</v>
-      </c>
-      <c r="D11">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>1152</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1168</v>
-      </c>
-      <c r="C12">
-        <v>175</v>
-      </c>
-      <c r="D12">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>1153</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C13">
-        <v>88</v>
-      </c>
-      <c r="D13">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C14">
-        <v>268</v>
-      </c>
-      <c r="D14">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C15">
-        <v>230</v>
-      </c>
-      <c r="D15">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C16">
-        <v>336</v>
-      </c>
-      <c r="D16">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C17">
-        <v>336</v>
-      </c>
-      <c r="D17">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>1155</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C18">
-        <v>55</v>
-      </c>
-      <c r="D18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C19">
-        <v>56</v>
-      </c>
-      <c r="D19">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>1157</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C20">
-        <v>40</v>
-      </c>
-      <c r="D20">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C21">
-        <v>118</v>
-      </c>
-      <c r="D21">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1144</v>
-      </c>
-      <c r="C22">
-        <v>364</v>
-      </c>
-      <c r="D22">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1144</v>
-      </c>
-      <c r="C23">
-        <v>332</v>
-      </c>
-      <c r="D23">
-        <v>264</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -12086,7 +12678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -12661,7 +13253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G33"/>
   <sheetViews>
@@ -13269,7 +13861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -13561,7 +14153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -13838,7 +14430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -14268,7 +14860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -14401,7 +14993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -14597,7 +15189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -14819,12 +15411,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C1">
+        <v>300</v>
+      </c>
+      <c r="D1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C2">
+        <v>128</v>
+      </c>
+      <c r="D2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C3">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14989,7 +15642,7 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -15105,82 +15758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1175</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C1">
-        <v>128</v>
-      </c>
-      <c r="D1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C2">
-        <v>122</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>798</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C4">
-        <v>370</v>
-      </c>
-      <c r="D4">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F7"/>
   <sheetViews>
@@ -15305,7 +15883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -15495,6 +16073,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C2">
+        <v>370</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -16096,7 +16721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -16726,7 +17351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -17323,7 +17948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -17806,7 +18431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -18119,587 +18744,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="22.77734375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="20.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D1" s="1">
-        <v>286</v>
-      </c>
-      <c r="E1" s="1">
-        <v>260</v>
-      </c>
-      <c r="F1" s="1">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="1">
-        <v>296</v>
-      </c>
-      <c r="E2" s="1">
-        <v>254</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="1">
-        <v>300</v>
-      </c>
-      <c r="E3" s="1">
-        <v>242</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="1">
-        <v>300</v>
-      </c>
-      <c r="E4" s="1">
-        <v>232</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" s="1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D5" s="1">
-        <v>297</v>
-      </c>
-      <c r="E5" s="1">
-        <v>228</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D6" s="1">
-        <v>294</v>
-      </c>
-      <c r="E6" s="1">
-        <v>224</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="1">
-        <v>294</v>
-      </c>
-      <c r="E7" s="1">
-        <v>216</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="1">
-        <v>294</v>
-      </c>
-      <c r="E8" s="1">
-        <v>208</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D9" s="1">
-        <v>294</v>
-      </c>
-      <c r="E9" s="1">
-        <v>200</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" s="1">
-        <v>294</v>
-      </c>
-      <c r="E10" s="1">
-        <v>192</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="1">
-        <v>290</v>
-      </c>
-      <c r="E11" s="1">
-        <v>182</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D12" s="1">
-        <v>284</v>
-      </c>
-      <c r="E12" s="1">
-        <v>176</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="1">
-        <v>278</v>
-      </c>
-      <c r="E13" s="1">
-        <v>172</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" s="1">
-        <v>271</v>
-      </c>
-      <c r="E14" s="1">
-        <v>172</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D15" s="1">
-        <v>265</v>
-      </c>
-      <c r="E15" s="1">
-        <v>172</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D16" s="1">
-        <v>258</v>
-      </c>
-      <c r="E16" s="1">
-        <v>172</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="1">
-        <v>251</v>
-      </c>
-      <c r="E17" s="1">
-        <v>172</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="1">
-        <v>240</v>
-      </c>
-      <c r="E18" s="1">
-        <v>164</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D19" s="1">
-        <v>234</v>
-      </c>
-      <c r="E19" s="1">
-        <v>156</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="1">
-        <v>234</v>
-      </c>
-      <c r="E20" s="1">
-        <v>150</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D21" s="1">
-        <v>231</v>
-      </c>
-      <c r="E21" s="1">
-        <v>145</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D22" s="1">
-        <v>227</v>
-      </c>
-      <c r="E22" s="1">
-        <v>141</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D23" s="1">
-        <v>222</v>
-      </c>
-      <c r="E23" s="1">
-        <v>136</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D24" s="1">
-        <v>218</v>
-      </c>
-      <c r="E24" s="1">
-        <v>128</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D25" s="1">
-        <v>218</v>
-      </c>
-      <c r="E25" s="1">
-        <v>119</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D26" s="1">
-        <v>212</v>
-      </c>
-      <c r="E26" s="1">
-        <v>116</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D27" s="1">
-        <v>205</v>
-      </c>
-      <c r="E27" s="1">
-        <v>116</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D28" s="1">
-        <v>198</v>
-      </c>
-      <c r="E28" s="1">
-        <v>116</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D29" s="1">
-        <v>192</v>
-      </c>
-      <c r="E29" s="1">
-        <v>120</v>
-      </c>
-      <c r="F29" s="1">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>